<commit_message>
UPD: exel and pptx - updated graphs
</commit_message>
<xml_diff>
--- a/sorts.xlsx
+++ b/sorts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="244" yWindow="111" windowWidth="14810" windowHeight="8020"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -140,8 +140,9 @@
               <c:idx val="0"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-683F-4364-A5A2-1174E14BBC9E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -149,8 +150,9 @@
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-683F-4364-A5A2-1174E14BBC9E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -158,8 +160,9 @@
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-683F-4364-A5A2-1174E14BBC9E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -167,8 +170,9 @@
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-683F-4364-A5A2-1174E14BBC9E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -232,10 +236,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$9</c:f>
+              <c:f>Лист1!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -251,13 +255,16 @@
                 <c:pt idx="4">
                   <c:v>100000</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
                   <c:v>1000000</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="7" formatCode="General">
                   <c:v>10000000</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="8" formatCode="General">
                   <c:v>100000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -265,10 +272,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$2:$B$6</c:f>
+              <c:f>Лист1!$B$2:$B$7</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -283,12 +290,15 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>15.656000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59.533999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-EEAA-4451-9BBD-28FDEA45335B}"/>
             </c:ext>
@@ -334,7 +344,7 @@
           </c:marker>
           <c:dLbls>
             <c:dLbl>
-              <c:idx val="5"/>
+              <c:idx val="6"/>
               <c:layout/>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
@@ -347,21 +357,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:layout/>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-683F-4364-A5A2-1174E14BBC9E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -378,6 +375,9 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-683F-4364-A5A2-1174E14BBC9E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -439,10 +439,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$9</c:f>
+              <c:f>Лист1!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -458,13 +458,16 @@
                 <c:pt idx="4">
                   <c:v>100000</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
                   <c:v>1000000</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="7" formatCode="General">
                   <c:v>10000000</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="8" formatCode="General">
                   <c:v>100000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -472,10 +475,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$C$2:$C$9</c:f>
+              <c:f>Лист1!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -492,19 +495,22 @@
                   <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>1.7000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>9.9000000000000005E-2</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1.0660000000000001</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>11.776999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-EEAA-4451-9BBD-28FDEA45335B}"/>
             </c:ext>
@@ -553,8 +559,9 @@
               <c:idx val="0"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-683F-4364-A5A2-1174E14BBC9E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -562,8 +569,9 @@
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-683F-4364-A5A2-1174E14BBC9E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -571,8 +579,9 @@
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-683F-4364-A5A2-1174E14BBC9E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -580,8 +589,9 @@
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-683F-4364-A5A2-1174E14BBC9E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -589,8 +599,21 @@
               <c:idx val="4"/>
               <c:delete val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-683F-4364-A5A2-1174E14BBC9E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-683F-4364-A5A2-1174E14BBC9E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -654,10 +677,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$D$2:$D$8</c:f>
+              <c:f>Лист1!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -674,23 +697,25 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>1.605</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>6.3</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>81.92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-EEAA-4451-9BBD-28FDEA45335B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -897,7 +922,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1558,14 +1583,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>72390</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>41909</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>422031</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>46892</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1586,16 +1611,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>179042</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>516666</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>102311</xdr:rowOff>
+      <xdr:rowOff>158582</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>-1</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>337624</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>67005</xdr:rowOff>
+      <xdr:rowOff>123276</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1612,8 +1637,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3708755" y="281355"/>
-          <a:ext cx="4117997" cy="2292257"/>
+          <a:off x="7782629" y="341462"/>
+          <a:ext cx="4153807" cy="2342134"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1912,16 +1937,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.296875" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -2009,32 +2034,46 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1000000</v>
+      <c r="A7" s="2">
+        <v>200000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>59.533999999999999</v>
       </c>
       <c r="C7">
-        <v>9.9000000000000005E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="D7">
-        <v>6.3</v>
+        <v>1.605</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>10000000</v>
+        <v>1000000</v>
       </c>
       <c r="C8">
-        <v>1.0660000000000001</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="D8">
-        <v>81.92</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
+        <v>10000000</v>
+      </c>
+      <c r="C9">
+        <v>1.0660000000000001</v>
+      </c>
+      <c r="D9">
+        <v>81.92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>100000000</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>11.776999999999999</v>
       </c>
     </row>

</xml_diff>